<commit_message>
Ludilo danasnje doradjeno (valjda je ok) ako nije nemojte mi spominjati familiju
</commit_message>
<xml_diff>
--- a/Ludiloo danasnje/RezervacijaKarataZaPravnoLiceIPlacanje.xlsx
+++ b/Ludiloo danasnje/RezervacijaKarataZaPravnoLiceIPlacanje.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ena\Desktop\OOAD Scenarij i tok\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Naziv:</t>
   </si>
@@ -44,9 +39,6 @@
     <t>Tok događaja:</t>
   </si>
   <si>
-    <t>Fizičko lice</t>
-  </si>
-  <si>
     <t>Multiplex Sveg</t>
   </si>
   <si>
@@ -62,18 +54,6 @@
     <t xml:space="preserve">Alternativni tok 1 </t>
   </si>
   <si>
-    <t>Korisnik ne prati proslijeđeni link.</t>
-  </si>
-  <si>
-    <t>1. Rezervacija ne prolazi verifikaciju zbog poslovnog pravila.</t>
-  </si>
-  <si>
-    <t>3. Brisanje do tada zabilježenih podataka.</t>
-  </si>
-  <si>
-    <t>2. Vraćanje na početnu stranicu.</t>
-  </si>
-  <si>
     <t>1. Pristupanje interfejsu za rezervaciju.</t>
   </si>
   <si>
@@ -83,18 +63,6 @@
     <t>Alternativni tok1 2:</t>
   </si>
   <si>
-    <t>Sistem za autorizaciju kartica nije odobrio transakciju</t>
-  </si>
-  <si>
-    <t>Na dvanaestom koraku glavnog toka nisu zadovoljeni uvjeti za nastavak rezervacije.</t>
-  </si>
-  <si>
-    <t>1. Rezervacija ne prolazi verifikaciju zbog sistema za autorizaciju.</t>
-  </si>
-  <si>
-    <t>Na jedanaestom koraku glavnog toka nije zadovoljeno poslovno pravilo da korisnik mora u roku od 15 minuta potvrditi e-mail.</t>
-  </si>
-  <si>
     <t>Scenario 4 i tok događaja</t>
   </si>
   <si>
@@ -150,13 +118,37 @@
   </si>
   <si>
     <t>13. Provjera identiteta</t>
+  </si>
+  <si>
+    <t>Korisnik je odabrao opciju plaćanja cjelokupnog iznosa</t>
+  </si>
+  <si>
+    <t>Korisnik je odabrao opciju plaćanja avansa</t>
+  </si>
+  <si>
+    <t>Na destom koraku glavnog toka, korisnik je izabrao opciju plaćanja avansa</t>
+  </si>
+  <si>
+    <t>Na desetom koraku glavnog toka, korisnik je izabrao opciju plaćanja cjelokupnog iznosa</t>
+  </si>
+  <si>
+    <t>1. Nakon utvrđivanja identiteta, pravno lice se obavještava o iznosu koji treba doplatiti</t>
+  </si>
+  <si>
+    <t>2. Doplaćuje iznos usluge</t>
+  </si>
+  <si>
+    <t>3. Pravnom licu se dodjeljuje ključ sale</t>
+  </si>
+  <si>
+    <t>1. Nakon utvrđivanja identiteta, pravnom licu se dodjeljuje ključ sale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,7 +458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,7 +493,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -678,280 +670,268 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" ht="31.5">
       <c r="A4" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="15"/>
     </row>
-    <row r="5" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="27.75" thickBot="1">
       <c r="A5" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B5" s="12"/>
     </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="183" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="229.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="41.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="41.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="39" customHeight="1" thickTop="1">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
       <c r="A12" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:2" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="26.25" customHeight="1" thickBot="1">
       <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="87" customHeight="1" thickBot="1">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="57" customHeight="1" thickBot="1">
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="70.5" customHeight="1" thickBot="1">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="55.5" customHeight="1" thickBot="1">
+      <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="55.5" customHeight="1" thickBot="1">
+      <c r="A18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2" ht="46.5" customHeight="1" thickBot="1">
+      <c r="A19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="46.5" customHeight="1" thickBot="1">
+      <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="21" spans="1:2" ht="57" customHeight="1"/>
+    <row r="22" spans="1:2" ht="27.75" thickBot="1">
+      <c r="A22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:2" ht="42.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:2" ht="48" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="29.25" customHeight="1" thickTop="1"/>
+    <row r="26" spans="1:2" ht="23.25" thickBot="1">
       <c r="A26" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="30" thickBot="1">
       <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:2" ht="51" customHeight="1" thickBot="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="51" customHeight="1"/>
+    <row r="30" spans="1:2" ht="27.75" thickBot="1">
+      <c r="A30" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:2" ht="24" thickTop="1" thickBot="1">
+      <c r="A31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="43.5" thickTop="1" thickBot="1">
+      <c r="A32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickTop="1"/>
+    <row r="34" spans="1:2" ht="23.25" thickBot="1">
+      <c r="A34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="13"/>
+    </row>
+    <row r="35" spans="1:2" ht="30" thickBot="1">
+      <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="12"/>
-    </row>
-    <row r="33" spans="1:2" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="13"/>
-    </row>
-    <row r="37" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:2" ht="42.75" thickBot="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="21.75" thickBot="1">
+      <c r="A37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="1:2" ht="21.75" thickBot="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B3"/>

</xml_diff>